<commit_message>
ER-Model überarbeitet Relationenmodel erstellt Stunden aufgezeichnet
18.07.2025 - Gabriel Deiac
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
+++ b/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\DA-Digitaler_Fluplatz\Digitales-Flugplatzmanagement\Stundenaufzeichnungen\Gabriel Deiac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9227699D-AA4A-448D-8BEF-F95524D78AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4BF163-9A3B-41DF-A784-AE0ACE3C07A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Stundenaufzeichnungen für Diplomarbeit</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve">Besprechung mit Julian </t>
+  </si>
+  <si>
+    <t>Besprechung mit Julian wegen Status Meeting am 19.07, Relationenmodel fertiggestellt und Er Model überarbeitet</t>
   </si>
 </sst>
 </file>
@@ -205,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -213,10 +216,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -556,7 +562,7 @@
   <dimension ref="A2:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,13 +612,13 @@
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="3" t="s">
         <v>4</v>
       </c>
@@ -722,14 +728,20 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="4"/>
+    <row r="18" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>45856</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -1003,16 +1015,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="10"/>
       <c r="G49" s="3">
         <f>SUM(G11:G48)</f>
-        <v>14.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1028,13 +1040,13 @@
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1050,7 +1062,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="4">
         <f>G49</f>
-        <v>14.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1460,7 +1472,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="10" t="s">
+      <c r="B99" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="6"/>
@@ -1469,83 +1481,11 @@
       <c r="F99" s="6"/>
       <c r="G99" s="3">
         <f>SUM(G53:G98)</f>
-        <v>14.5</v>
+        <v>17.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B49:F49"/>
@@ -1562,6 +1502,78 @@
     <mergeCell ref="B88:F88"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1570,18 +1582,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1729,6 +1741,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AF60E-0EF1-43CF-BBE9-09CB79E28327}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1741,14 +1761,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AF60E-0EF1-43CF-BBE9-09CB79E28327}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Prtokoll Entwurf für Besprechung am 31.07, Zeit 25.07.2025 - Gabriel Deiac
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
+++ b/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\DA-Digitaler_Fluplatz\Digitales-Flugplatzmanagement\Stundenaufzeichnungen\Gabriel Deiac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB9A1B0-D8DE-4FF6-ABD3-698A9800E4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB674BC5-07F6-4D41-91D6-6AC53A66F9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Stundenaufzeichnungen für Diplomarbeit</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Email Zwischenstand mit Julian schreiben</t>
+  </si>
+  <si>
+    <t>Beprechungsprotokoll Entwurf für morgen fertiggestellt, Themen ausgemacht</t>
   </si>
 </sst>
 </file>
@@ -228,13 +231,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -573,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:F22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,13 +627,13 @@
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="3" t="s">
         <v>4</v>
       </c>
@@ -744,13 +747,13 @@
       <c r="A18" s="5">
         <v>45856</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="4">
         <v>3</v>
       </c>
@@ -816,13 +819,19 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="5">
+        <v>45868</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
@@ -1051,16 +1060,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="11"/>
       <c r="G49" s="3">
         <f>SUM(G11:G48)</f>
-        <v>22.25</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,13 +1085,13 @@
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1107,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="4">
         <f>G49</f>
-        <v>22.25</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1508,7 +1517,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="10" t="s">
+      <c r="B99" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="6"/>
@@ -1517,83 +1526,11 @@
       <c r="F99" s="6"/>
       <c r="G99" s="3">
         <f>SUM(G53:G98)</f>
-        <v>22.25</v>
+        <v>22.75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B49:F49"/>
@@ -1610,6 +1547,78 @@
     <mergeCell ref="B88:F88"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1618,6 +1627,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010094CA166A05CDA845ABC57209B279665E" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="5ec4c24f54434c3ab0c7f6bcef77c0a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4aace298-5e4d-42df-b8b1-113942a4c769" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d1de0c83e350131cff9e66f69627781" ns2:_="">
     <xsd:import namespace="4aace298-5e4d-42df-b8b1-113942a4c769"/>
@@ -1761,12 +1776,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1777,6 +1786,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f99cb733-4833-4ade-8692-0877df31b8bf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5CC49F-06EC-4375-8D15-91BBCFC1D049}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1794,23 +1820,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f99cb733-4833-4ade-8692-0877df31b8bf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AF60E-0EF1-43CF-BBE9-09CB79E28327}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Protoklle und Projekplanung Vorlagen hinzugefügt, Zeit
31.07.2025 - Gabriel Deiac
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
+++ b/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\DA-Digitaler_Fluplatz\Digitales-Flugplatzmanagement\Stundenaufzeichnungen\Gabriel Deiac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB674BC5-07F6-4D41-91D6-6AC53A66F9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8B9AEB-C6F4-4F4A-B02F-7694DD4BAB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Stundenaufzeichnungen für Diplomarbeit</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Beprechungsprotokoll Entwurf für morgen fertiggestellt, Themen ausgemacht</t>
+  </si>
+  <si>
+    <t>Besprechung mit Prof Schatz und Bespr. Protokoll schreiben</t>
   </si>
 </sst>
 </file>
@@ -231,13 +234,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -576,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,13 +630,13 @@
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="3" t="s">
         <v>4</v>
       </c>
@@ -747,13 +750,13 @@
       <c r="A18" s="5">
         <v>45856</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="4">
         <v>3</v>
       </c>
@@ -834,13 +837,19 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="5">
+        <v>45869</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
@@ -1060,16 +1069,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="11"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="9"/>
       <c r="G49" s="3">
         <f>SUM(G11:G48)</f>
-        <v>22.75</v>
+        <v>24.25</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1085,13 +1094,13 @@
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
       <c r="G52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1107,7 +1116,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="4">
         <f>G49</f>
-        <v>22.75</v>
+        <v>24.25</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1517,7 +1526,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="7" t="s">
+      <c r="B99" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="6"/>
@@ -1526,11 +1535,83 @@
       <c r="F99" s="6"/>
       <c r="G99" s="3">
         <f>SUM(G53:G98)</f>
-        <v>22.75</v>
+        <v>24.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B49:F49"/>
@@ -1547,78 +1628,6 @@
     <mergeCell ref="B88:F88"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1627,12 +1636,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010094CA166A05CDA845ABC57209B279665E" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="5ec4c24f54434c3ab0c7f6bcef77c0a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4aace298-5e4d-42df-b8b1-113942a4c769" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d1de0c83e350131cff9e66f69627781" ns2:_="">
     <xsd:import namespace="4aace298-5e4d-42df-b8b1-113942a4c769"/>
@@ -1776,6 +1779,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1786,23 +1795,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f99cb733-4833-4ade-8692-0877df31b8bf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5CC49F-06EC-4375-8D15-91BBCFC1D049}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1820,6 +1812,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f99cb733-4833-4ade-8692-0877df31b8bf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AF60E-0EF1-43CF-BBE9-09CB79E28327}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Arbeitspakete definiert, Projekthandbuch Vorlage erstellt, Zeit
02.08.2025 - Gabriel Deiac
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
+++ b/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\DA-Digitaler_Fluplatz\Digitales-Flugplatzmanagement\Stundenaufzeichnungen\Gabriel Deiac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8B9AEB-C6F4-4F4A-B02F-7694DD4BAB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27108D6-FC70-4843-A81B-E4940B27A787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Stundenaufzeichnungen für Diplomarbeit</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Besprechung mit Prof Schatz und Bespr. Protokoll schreiben</t>
+  </si>
+  <si>
+    <t>Testdaten und Entwurf DB erstellen</t>
+  </si>
+  <si>
+    <t>Arbeitspakete definiert</t>
   </si>
 </sst>
 </file>
@@ -580,7 +586,7 @@
   <dimension ref="A2:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B32" activeCellId="1" sqref="B26:F26 B32:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,22 +858,34 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="5">
+        <v>45869</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="5">
+        <v>45718</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
@@ -1078,7 +1096,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="3">
         <f>SUM(G11:G48)</f>
-        <v>24.25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1116,7 +1134,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="4">
         <f>G49</f>
-        <v>24.25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1535,7 +1553,7 @@
       <c r="F99" s="6"/>
       <c r="G99" s="3">
         <f>SUM(G53:G98)</f>
-        <v>24.25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gantt und Entwürfe hinzufügen
06.08.2025 - Gabriel Deiac
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
+++ b/Stundenaufzeichnungen/Gabriel Deiac/DA_Stundenaufzeichnungen-GabrielDeiac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\DA-Digitaler_Fluplatz\Digitales-Flugplatzmanagement\Stundenaufzeichnungen\Gabriel Deiac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D1AE4B-C9C6-4C7D-9593-74E721B103D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3306C8F-385D-410C-83DD-41087B5E8AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Stundenaufzeichnungen für Diplomarbeit</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Arbeitspakete fertiggestellt</t>
+  </si>
+  <si>
+    <t>Gantt Prototyp erstellt</t>
   </si>
 </sst>
 </file>
@@ -243,13 +246,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -588,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:F30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,13 +642,13 @@
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="3" t="s">
         <v>4</v>
       </c>
@@ -759,13 +762,13 @@
       <c r="A18" s="5">
         <v>45856</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="4">
         <v>3</v>
       </c>
@@ -906,13 +909,19 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="5">
+        <v>45875</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="4"/>
+      <c r="G28" s="4">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
@@ -1096,16 +1105,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="11"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="9"/>
       <c r="G49" s="3">
         <f>SUM(G11:G48)</f>
-        <v>28.25</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1121,13 +1130,13 @@
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
       <c r="G52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1143,7 +1152,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="4">
         <f>G49</f>
-        <v>28.25</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1553,7 +1562,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="7" t="s">
+      <c r="B99" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="6"/>
@@ -1562,11 +1571,83 @@
       <c r="F99" s="6"/>
       <c r="G99" s="3">
         <f>SUM(G53:G98)</f>
-        <v>28.25</v>
+        <v>29.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B49:F49"/>
@@ -1583,78 +1664,6 @@
     <mergeCell ref="B88:F88"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1663,12 +1672,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010094CA166A05CDA845ABC57209B279665E" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="5ec4c24f54434c3ab0c7f6bcef77c0a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4aace298-5e4d-42df-b8b1-113942a4c769" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d1de0c83e350131cff9e66f69627781" ns2:_="">
     <xsd:import namespace="4aace298-5e4d-42df-b8b1-113942a4c769"/>
@@ -1812,6 +1815,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1822,23 +1831,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f99cb733-4833-4ade-8692-0877df31b8bf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5CC49F-06EC-4375-8D15-91BBCFC1D049}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1856,6 +1848,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f99cb733-4833-4ade-8692-0877df31b8bf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AF60E-0EF1-43CF-BBE9-09CB79E28327}">
   <ds:schemaRefs>

</xml_diff>